<commit_message>
EPBDS-5325 Saved a component type in a result array
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="977" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="518">
   <si>
     <t>Tests to test rules helper methods for Max and Min value of different types</t>
   </si>
@@ -1583,6 +1583,15 @@
   </si>
   <si>
     <t>return getValues("ABC");</t>
+  </si>
+  <si>
+    <t>Datatype Primes &lt;Integer&gt;</t>
+  </si>
+  <si>
+    <t>Method Object[] testGetValuesPrimesAlias()</t>
+  </si>
+  <si>
+    <t>return getValues(Primes);</t>
   </si>
 </sst>
 </file>
@@ -1784,17 +1793,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
@@ -2195,19 +2204,19 @@
       <c r="D1" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="15"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
@@ -2216,10 +2225,10 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="15"/>
+      <c r="G6" s="19"/>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2312,10 +2321,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="15"/>
+      <c r="D14" s="19"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
@@ -2324,10 +2333,10 @@
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="15"/>
+      <c r="G15" s="19"/>
       <c r="I15" s="2" t="s">
         <v>21</v>
       </c>
@@ -2420,10 +2429,10 @@
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="15"/>
+      <c r="D23" s="19"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
@@ -2432,10 +2441,10 @@
       <c r="D24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="15"/>
+      <c r="G24" s="19"/>
       <c r="I24" s="2" t="s">
         <v>30</v>
       </c>
@@ -2520,10 +2529,10 @@
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="15"/>
+      <c r="D32" s="19"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
@@ -2532,10 +2541,10 @@
       <c r="D33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="15"/>
+      <c r="G33" s="19"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
@@ -2608,10 +2617,10 @@
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="15"/>
+      <c r="D41" s="19"/>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
@@ -2620,10 +2629,10 @@
       <c r="D42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="G42" s="15"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
@@ -2696,10 +2705,10 @@
       </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="15"/>
+      <c r="D50" s="19"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
@@ -2708,10 +2717,10 @@
       <c r="D51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F51" s="15" t="s">
+      <c r="F51" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G51" s="15"/>
+      <c r="G51" s="19"/>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
@@ -2784,19 +2793,19 @@
       </c>
     </row>
     <row r="60" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C60" s="16" t="s">
+      <c r="C60" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D60" s="16"/>
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="16"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="15" t="s">
+      <c r="C62" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D62" s="15"/>
+      <c r="D62" s="19"/>
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
@@ -2805,10 +2814,10 @@
       <c r="D63" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="15" t="s">
+      <c r="F63" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="G63" s="15"/>
+      <c r="G63" s="19"/>
       <c r="I63" s="2" t="s">
         <v>49</v>
       </c>
@@ -2901,10 +2910,10 @@
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C71" s="15" t="s">
+      <c r="C71" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D71" s="15"/>
+      <c r="D71" s="19"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
@@ -2913,10 +2922,10 @@
       <c r="D72" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F72" s="15" t="s">
+      <c r="F72" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="G72" s="15"/>
+      <c r="G72" s="19"/>
       <c r="I72" s="2" t="s">
         <v>56</v>
       </c>
@@ -3009,10 +3018,10 @@
       </c>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C80" s="15" t="s">
+      <c r="C80" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="D80" s="15"/>
+      <c r="D80" s="19"/>
     </row>
     <row r="81" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C81" s="1" t="s">
@@ -3021,10 +3030,10 @@
       <c r="D81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F81" s="15" t="s">
+      <c r="F81" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="G81" s="15"/>
+      <c r="G81" s="19"/>
       <c r="I81" s="2" t="s">
         <v>61</v>
       </c>
@@ -3109,10 +3118,10 @@
       </c>
     </row>
     <row r="89" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C89" s="15" t="s">
+      <c r="C89" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="D89" s="15"/>
+      <c r="D89" s="19"/>
     </row>
     <row r="90" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C90" s="1" t="s">
@@ -3121,10 +3130,10 @@
       <c r="D90" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F90" s="15" t="s">
+      <c r="F90" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="G90" s="15"/>
+      <c r="G90" s="19"/>
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C91" s="1" t="s">
@@ -3197,10 +3206,10 @@
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C98" s="15" t="s">
+      <c r="C98" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D98" s="15"/>
+      <c r="D98" s="19"/>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
@@ -3209,10 +3218,10 @@
       <c r="D99" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F99" s="15" t="s">
+      <c r="F99" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="G99" s="15"/>
+      <c r="G99" s="19"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C100" s="1" t="s">
@@ -3285,10 +3294,10 @@
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C107" s="15" t="s">
+      <c r="C107" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="D107" s="15"/>
+      <c r="D107" s="19"/>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" s="1" t="s">
@@ -3297,10 +3306,10 @@
       <c r="D108" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F108" s="15" t="s">
+      <c r="F108" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="G108" s="15"/>
+      <c r="G108" s="19"/>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C109" s="1" t="s">
@@ -3374,26 +3383,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="C80:D80"/>
     <mergeCell ref="C107:D107"/>
     <mergeCell ref="F108:G108"/>
     <mergeCell ref="F81:G81"/>
@@ -3401,6 +3390,26 @@
     <mergeCell ref="F90:G90"/>
     <mergeCell ref="C98:D98"/>
     <mergeCell ref="F99:G99"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -6043,10 +6052,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B25"/>
+  <dimension ref="B2:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6056,7 +6065,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="15" t="s">
         <v>503</v>
       </c>
     </row>
@@ -6106,22 +6115,22 @@
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="16" t="s">
         <v>508</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="16" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="16" t="s">
         <v>506</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="16" t="s">
         <v>505</v>
       </c>
     </row>
@@ -6143,6 +6152,41 @@
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
         <v>514</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="13">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="10" t="s">
+        <v>517</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-5740 Fixed getvalues method
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" firstSheet="14" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" firstSheet="10" activeTab="24"/>
   </bookViews>
   <sheets>
     <sheet name="MaxMinTests" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="980" uniqueCount="518">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="507">
   <si>
     <t>Tests to test rules helper methods for Max and Min value of different types</t>
   </si>
@@ -1531,42 +1531,15 @@
     <t>Method Object[] testFlatten(Object[] data)</t>
   </si>
   <si>
-    <t>Data String agency</t>
-  </si>
-  <si>
-    <t>this</t>
-  </si>
-  <si>
-    <t>Agency</t>
-  </si>
-  <si>
-    <t>return getValues(agency);</t>
-  </si>
-  <si>
     <t>Method Object[] testGetValuesAlias()</t>
   </si>
   <si>
-    <t>Method Object[] testGetValuesData()</t>
-  </si>
-  <si>
     <t>Datatype Agency &lt;String&gt;</t>
   </si>
   <si>
     <t>return getValues(Agency);</t>
   </si>
   <si>
-    <t>Data4</t>
-  </si>
-  <si>
-    <t>Data0</t>
-  </si>
-  <si>
-    <t>Data2</t>
-  </si>
-  <si>
-    <t>Data1</t>
-  </si>
-  <si>
     <t>Alias1</t>
   </si>
   <si>
@@ -1577,12 +1550,6 @@
   </si>
   <si>
     <t>Alias4</t>
-  </si>
-  <si>
-    <t>Method Object[] testGetValuesWrongType()</t>
-  </si>
-  <si>
-    <t>return getValues("ABC");</t>
   </si>
   <si>
     <t>Datatype Primes &lt;Integer&gt;</t>
@@ -1598,21 +1565,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1768,50 +1727,48 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% - Акцент5" xfId="2" builtinId="46"/>
-    <cellStyle name="40% - Акцент1" xfId="1" builtinId="31"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1892,9 +1849,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1932,7 +1889,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2004,7 +1961,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2199,27 +2156,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="17"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
@@ -2228,10 +2185,10 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="F6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="17"/>
+      <c r="G6" s="16"/>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2324,10 +2281,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="17"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
@@ -2336,10 +2293,10 @@
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="17"/>
+      <c r="G15" s="16"/>
       <c r="I15" s="2" t="s">
         <v>21</v>
       </c>
@@ -2432,10 +2389,10 @@
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="17"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
@@ -2444,10 +2401,10 @@
       <c r="D24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="17" t="s">
+      <c r="F24" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="17"/>
+      <c r="G24" s="16"/>
       <c r="I24" s="2" t="s">
         <v>30</v>
       </c>
@@ -2532,10 +2489,10 @@
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="17" t="s">
+      <c r="C32" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="17"/>
+      <c r="D32" s="16"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
@@ -2544,10 +2501,10 @@
       <c r="D33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="17" t="s">
+      <c r="F33" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="17"/>
+      <c r="G33" s="16"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
@@ -2620,10 +2577,10 @@
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="17" t="s">
+      <c r="C41" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="17"/>
+      <c r="D41" s="16"/>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
@@ -2632,10 +2589,10 @@
       <c r="D42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="F42" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G42" s="17"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
@@ -2708,10 +2665,10 @@
       </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C50" s="17" t="s">
+      <c r="C50" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="17"/>
+      <c r="D50" s="16"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
@@ -2720,10 +2677,10 @@
       <c r="D51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F51" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="G51" s="17"/>
+      <c r="G51" s="16"/>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
@@ -2796,19 +2753,19 @@
       </c>
     </row>
     <row r="60" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C60" s="18" t="s">
+      <c r="C60" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
+      <c r="F60" s="17"/>
+      <c r="G60" s="17"/>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="17" t="s">
+      <c r="C62" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D62" s="17"/>
+      <c r="D62" s="16"/>
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
@@ -2817,10 +2774,10 @@
       <c r="D63" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="17" t="s">
+      <c r="F63" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G63" s="17"/>
+      <c r="G63" s="16"/>
       <c r="I63" s="2" t="s">
         <v>49</v>
       </c>
@@ -2913,10 +2870,10 @@
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C71" s="17" t="s">
+      <c r="C71" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D71" s="17"/>
+      <c r="D71" s="16"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
@@ -2925,10 +2882,10 @@
       <c r="D72" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F72" s="17" t="s">
+      <c r="F72" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G72" s="17"/>
+      <c r="G72" s="16"/>
       <c r="I72" s="2" t="s">
         <v>56</v>
       </c>
@@ -3021,10 +2978,10 @@
       </c>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C80" s="17" t="s">
+      <c r="C80" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D80" s="17"/>
+      <c r="D80" s="16"/>
     </row>
     <row r="81" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C81" s="1" t="s">
@@ -3033,10 +2990,10 @@
       <c r="D81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F81" s="17" t="s">
+      <c r="F81" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G81" s="17"/>
+      <c r="G81" s="16"/>
       <c r="I81" s="2" t="s">
         <v>61</v>
       </c>
@@ -3121,10 +3078,10 @@
       </c>
     </row>
     <row r="89" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C89" s="17" t="s">
+      <c r="C89" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D89" s="17"/>
+      <c r="D89" s="16"/>
     </row>
     <row r="90" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C90" s="1" t="s">
@@ -3133,10 +3090,10 @@
       <c r="D90" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F90" s="17" t="s">
+      <c r="F90" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G90" s="17"/>
+      <c r="G90" s="16"/>
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C91" s="1" t="s">
@@ -3209,10 +3166,10 @@
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C98" s="17" t="s">
+      <c r="C98" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D98" s="17"/>
+      <c r="D98" s="16"/>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
@@ -3221,10 +3178,10 @@
       <c r="D99" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F99" s="17" t="s">
+      <c r="F99" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G99" s="17"/>
+      <c r="G99" s="16"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C100" s="1" t="s">
@@ -3297,10 +3254,10 @@
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C107" s="17" t="s">
+      <c r="C107" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D107" s="17"/>
+      <c r="D107" s="16"/>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" s="1" t="s">
@@ -3309,10 +3266,10 @@
       <c r="D108" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F108" s="17" t="s">
+      <c r="F108" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G108" s="17"/>
+      <c r="G108" s="16"/>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C109" s="1" t="s">
@@ -3437,12 +3394,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -3571,12 +3528,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
@@ -5139,12 +5096,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -6030,7 +5987,7 @@
   <dimension ref="B2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6055,10 +6012,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B35"/>
+  <dimension ref="B2:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6068,128 +6025,73 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="15" t="s">
-        <v>503</v>
+      <c r="B2" s="14" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>509</v>
+        <v>500</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>510</v>
+        <v>501</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>511</v>
+        <v>502</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>512</v>
+        <v>503</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
-        <v>504</v>
+      <c r="B9" s="15" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
-        <v>498</v>
+      <c r="B14" s="13">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
-        <v>499</v>
+      <c r="B15" s="13">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
-        <v>508</v>
+      <c r="B16" s="13">
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+      <c r="B17" s="13">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="10" t="s">
         <v>506</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="15" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B29" s="13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B30" s="13">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="13">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B32" s="13">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="9" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="10" t="s">
-        <v>517</v>
       </c>
     </row>
   </sheetData>
@@ -6216,12 +6118,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -6483,12 +6385,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -6738,12 +6640,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
@@ -6915,12 +6817,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
@@ -7125,12 +7027,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">

</xml_diff>

<commit_message>
EPBDS-6101 Add operator intanceOf(object, Class)
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" firstSheet="10" activeTab="24"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" firstSheet="10" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="MaxMinTests" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="509">
   <si>
     <t>Tests to test rules helper methods for Max and Min value of different types</t>
   </si>
@@ -1559,6 +1559,12 @@
   </si>
   <si>
     <t>return getValues(Primes);</t>
+  </si>
+  <si>
+    <t>Method Boolean testInstanceOf(Long a)</t>
+  </si>
+  <si>
+    <t>return instanceOf(a, Number.class);</t>
   </si>
 </sst>
 </file>
@@ -1755,20 +1761,20 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Акцент5" xfId="2" builtinId="46"/>
+    <cellStyle name="40% - Акцент1" xfId="1" builtinId="31"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1849,9 +1855,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1889,7 +1895,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1961,7 +1967,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2156,12 +2162,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="17" t="s">
@@ -2173,10 +2179,10 @@
       <c r="G3" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
@@ -2185,10 +2191,10 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="18"/>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2281,10 +2287,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
@@ -2293,10 +2299,10 @@
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="16"/>
+      <c r="G15" s="18"/>
       <c r="I15" s="2" t="s">
         <v>21</v>
       </c>
@@ -2389,10 +2395,10 @@
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="16"/>
+      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
@@ -2401,10 +2407,10 @@
       <c r="D24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="16"/>
+      <c r="G24" s="18"/>
       <c r="I24" s="2" t="s">
         <v>30</v>
       </c>
@@ -2489,10 +2495,10 @@
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="16"/>
+      <c r="D32" s="18"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
@@ -2501,10 +2507,10 @@
       <c r="D33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="16"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
@@ -2577,10 +2583,10 @@
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="16"/>
+      <c r="D41" s="18"/>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
@@ -2589,10 +2595,10 @@
       <c r="D42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="16" t="s">
+      <c r="F42" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G42" s="16"/>
+      <c r="G42" s="18"/>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
@@ -2665,10 +2671,10 @@
       </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="16"/>
+      <c r="D50" s="18"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
@@ -2677,10 +2683,10 @@
       <c r="D51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F51" s="16" t="s">
+      <c r="F51" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="G51" s="16"/>
+      <c r="G51" s="18"/>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
@@ -2762,10 +2768,10 @@
       <c r="G60" s="17"/>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D62" s="16"/>
+      <c r="D62" s="18"/>
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
@@ -2774,10 +2780,10 @@
       <c r="D63" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="16" t="s">
+      <c r="F63" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G63" s="16"/>
+      <c r="G63" s="18"/>
       <c r="I63" s="2" t="s">
         <v>49</v>
       </c>
@@ -2870,10 +2876,10 @@
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C71" s="16" t="s">
+      <c r="C71" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D71" s="16"/>
+      <c r="D71" s="18"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
@@ -2882,10 +2888,10 @@
       <c r="D72" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F72" s="16" t="s">
+      <c r="F72" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G72" s="16"/>
+      <c r="G72" s="18"/>
       <c r="I72" s="2" t="s">
         <v>56</v>
       </c>
@@ -2978,10 +2984,10 @@
       </c>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C80" s="16" t="s">
+      <c r="C80" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D80" s="16"/>
+      <c r="D80" s="18"/>
     </row>
     <row r="81" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C81" s="1" t="s">
@@ -2990,10 +2996,10 @@
       <c r="D81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F81" s="16" t="s">
+      <c r="F81" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="G81" s="16"/>
+      <c r="G81" s="18"/>
       <c r="I81" s="2" t="s">
         <v>61</v>
       </c>
@@ -3078,10 +3084,10 @@
       </c>
     </row>
     <row r="89" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C89" s="16" t="s">
+      <c r="C89" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D89" s="16"/>
+      <c r="D89" s="18"/>
     </row>
     <row r="90" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C90" s="1" t="s">
@@ -3090,10 +3096,10 @@
       <c r="D90" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F90" s="16" t="s">
+      <c r="F90" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G90" s="16"/>
+      <c r="G90" s="18"/>
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C91" s="1" t="s">
@@ -3166,10 +3172,10 @@
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C98" s="16" t="s">
+      <c r="C98" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D98" s="16"/>
+      <c r="D98" s="18"/>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
@@ -3178,10 +3184,10 @@
       <c r="D99" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F99" s="16" t="s">
+      <c r="F99" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="G99" s="16"/>
+      <c r="G99" s="18"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C100" s="1" t="s">
@@ -3254,10 +3260,10 @@
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C107" s="16" t="s">
+      <c r="C107" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D107" s="16"/>
+      <c r="D107" s="18"/>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" s="1" t="s">
@@ -3266,10 +3272,10 @@
       <c r="D108" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F108" s="16" t="s">
+      <c r="F108" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="G108" s="16"/>
+      <c r="G108" s="18"/>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C109" s="1" t="s">
@@ -3343,26 +3349,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="C80:D80"/>
     <mergeCell ref="C107:D107"/>
     <mergeCell ref="F108:G108"/>
     <mergeCell ref="F81:G81"/>
@@ -3370,6 +3356,26 @@
     <mergeCell ref="F90:G90"/>
     <mergeCell ref="C98:D98"/>
     <mergeCell ref="F99:G99"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3394,12 +3400,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -3528,12 +3534,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
@@ -4363,10 +4369,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B19"/>
+  <dimension ref="B3:B22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4434,6 +4440,16 @@
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>343</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="10" t="s">
+        <v>508</v>
       </c>
     </row>
   </sheetData>
@@ -5096,12 +5112,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -6014,7 +6030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -6118,12 +6134,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -6385,12 +6401,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -6640,12 +6656,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
@@ -6817,12 +6833,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
@@ -7027,12 +7043,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">

</xml_diff>

<commit_message>
EPBDS-6913 Move allTrue(), anyTrue(), allFalse(), anyFalse() to the special 'util' module
Added tests, unified behavior for null and empty values, consolidated functionality in one place.
Removed deprecated xor() methods.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="500">
   <si>
     <t>Tests to test rules helper methods for Max and Min value of different types</t>
   </si>
@@ -1046,33 +1046,6 @@
   </si>
   <si>
     <t>Method BigDecimal testBigDecimalProduct(BigDecimal[] inputArray)</t>
-  </si>
-  <si>
-    <t>Method boolean testBoolTypeAllTrue(boolean[] inputArray)</t>
-  </si>
-  <si>
-    <t>return allTrue(inputArray);</t>
-  </si>
-  <si>
-    <t>Method Boolean testBoolAllTrue(Boolean[] inputArray)</t>
-  </si>
-  <si>
-    <t>Method boolean testBoolTypeXor(boolean[] inputArray)</t>
-  </si>
-  <si>
-    <t>return xor(inputArray);</t>
-  </si>
-  <si>
-    <t>Method Boolean testBoolXor(Boolean[] inputArray)</t>
-  </si>
-  <si>
-    <t>Method boolean testBoolTypeAnyTrue(boolean[] inputArray)</t>
-  </si>
-  <si>
-    <t>return anyTrue(inputArray);</t>
-  </si>
-  <si>
-    <t>Method Boolean testBoolAnyTrue(Boolean[] inputArray)</t>
   </si>
   <si>
     <t>Method long testDoubleTypeRound(double num)</t>
@@ -1761,20 +1734,20 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% - Акцент5" xfId="2" builtinId="46"/>
-    <cellStyle name="40% - Акцент1" xfId="1" builtinId="31"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1855,9 +1828,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1895,7 +1868,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1967,7 +1940,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2162,12 +2135,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="17" t="s">
@@ -2179,10 +2152,10 @@
       <c r="G3" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
@@ -2191,10 +2164,10 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="16"/>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2287,10 +2260,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="18"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
@@ -2299,10 +2272,10 @@
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="18"/>
+      <c r="G15" s="16"/>
       <c r="I15" s="2" t="s">
         <v>21</v>
       </c>
@@ -2395,10 +2368,10 @@
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="18"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
@@ -2407,10 +2380,10 @@
       <c r="D24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="18"/>
+      <c r="G24" s="16"/>
       <c r="I24" s="2" t="s">
         <v>30</v>
       </c>
@@ -2495,10 +2468,10 @@
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" s="16"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
@@ -2507,10 +2480,10 @@
       <c r="D33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="18"/>
+      <c r="G33" s="16"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
@@ -2583,10 +2556,10 @@
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="18"/>
+      <c r="D41" s="16"/>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
@@ -2595,10 +2568,10 @@
       <c r="D42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="F42" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G42" s="18"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
@@ -2671,10 +2644,10 @@
       </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="18"/>
+      <c r="D50" s="16"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
@@ -2683,10 +2656,10 @@
       <c r="D51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F51" s="18" t="s">
+      <c r="F51" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="G51" s="18"/>
+      <c r="G51" s="16"/>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
@@ -2768,10 +2741,10 @@
       <c r="G60" s="17"/>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D62" s="18"/>
+      <c r="D62" s="16"/>
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
@@ -2780,10 +2753,10 @@
       <c r="D63" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="18" t="s">
+      <c r="F63" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G63" s="18"/>
+      <c r="G63" s="16"/>
       <c r="I63" s="2" t="s">
         <v>49</v>
       </c>
@@ -2876,10 +2849,10 @@
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C71" s="18" t="s">
+      <c r="C71" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D71" s="18"/>
+      <c r="D71" s="16"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
@@ -2888,10 +2861,10 @@
       <c r="D72" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F72" s="18" t="s">
+      <c r="F72" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G72" s="18"/>
+      <c r="G72" s="16"/>
       <c r="I72" s="2" t="s">
         <v>56</v>
       </c>
@@ -2984,10 +2957,10 @@
       </c>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C80" s="18" t="s">
+      <c r="C80" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D80" s="18"/>
+      <c r="D80" s="16"/>
     </row>
     <row r="81" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C81" s="1" t="s">
@@ -2996,10 +2969,10 @@
       <c r="D81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F81" s="18" t="s">
+      <c r="F81" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G81" s="18"/>
+      <c r="G81" s="16"/>
       <c r="I81" s="2" t="s">
         <v>61</v>
       </c>
@@ -3084,10 +3057,10 @@
       </c>
     </row>
     <row r="89" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C89" s="18" t="s">
+      <c r="C89" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D89" s="18"/>
+      <c r="D89" s="16"/>
     </row>
     <row r="90" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C90" s="1" t="s">
@@ -3096,10 +3069,10 @@
       <c r="D90" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F90" s="18" t="s">
+      <c r="F90" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G90" s="18"/>
+      <c r="G90" s="16"/>
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C91" s="1" t="s">
@@ -3172,10 +3145,10 @@
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C98" s="18" t="s">
+      <c r="C98" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D98" s="18"/>
+      <c r="D98" s="16"/>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
@@ -3184,10 +3157,10 @@
       <c r="D99" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F99" s="18" t="s">
+      <c r="F99" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G99" s="18"/>
+      <c r="G99" s="16"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C100" s="1" t="s">
@@ -3260,10 +3233,10 @@
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C107" s="18" t="s">
+      <c r="C107" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D107" s="18"/>
+      <c r="D107" s="16"/>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" s="1" t="s">
@@ -3272,10 +3245,10 @@
       <c r="D108" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F108" s="18" t="s">
+      <c r="F108" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G108" s="18"/>
+      <c r="G108" s="16"/>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C109" s="1" t="s">
@@ -3349,6 +3322,26 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="C80:D80"/>
     <mergeCell ref="C107:D107"/>
     <mergeCell ref="F108:G108"/>
     <mergeCell ref="F81:G81"/>
@@ -3356,26 +3349,6 @@
     <mergeCell ref="F90:G90"/>
     <mergeCell ref="C98:D98"/>
     <mergeCell ref="F99:G99"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3400,12 +3373,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>215</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -3534,12 +3507,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>229</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
@@ -4369,87 +4342,25 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B22"/>
+  <dimension ref="B3:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125"/>
     <col min="2" max="2" width="49.28515625"/>
-    <col min="3" max="1025" width="11.5703125"/>
+    <col min="3" max="1012" width="11.5703125"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>336</v>
+        <v>498</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="10" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B15" s="9" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B22" s="10" t="s">
-        <v>508</v>
+        <v>499</v>
       </c>
     </row>
   </sheetData>
@@ -4479,92 +4390,92 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -4596,162 +4507,162 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
-        <v>365</v>
+        <v>356</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>366</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>367</v>
+        <v>358</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>368</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>369</v>
+        <v>360</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>370</v>
+        <v>361</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>371</v>
+        <v>362</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>373</v>
+        <v>364</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>374</v>
+        <v>365</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>377</v>
+        <v>368</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>378</v>
+        <v>369</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
     </row>
   </sheetData>
@@ -4783,186 +4694,186 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>379</v>
+        <v>370</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>380</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>383</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
-        <v>400</v>
+        <v>391</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
-        <v>401</v>
+        <v>392</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="9" t="s">
-        <v>402</v>
+        <v>393</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -4992,92 +4903,92 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>403</v>
+        <v>394</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>405</v>
+        <v>396</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>407</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>408</v>
+        <v>399</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>409</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>410</v>
+        <v>401</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>411</v>
+        <v>402</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>412</v>
+        <v>403</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>404</v>
+        <v>395</v>
       </c>
     </row>
   </sheetData>
@@ -5112,12 +5023,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -5335,146 +5246,146 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>413</v>
+        <v>404</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>414</v>
+        <v>405</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>420</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>421</v>
+        <v>412</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>422</v>
+        <v>413</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>427</v>
+        <v>418</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>428</v>
+        <v>419</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>429</v>
+        <v>420</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>430</v>
+        <v>421</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>431</v>
+        <v>422</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>432</v>
+        <v>423</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
     </row>
   </sheetData>
@@ -5504,112 +5415,112 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>435</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>436</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>437</v>
+        <v>428</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>438</v>
+        <v>429</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>439</v>
+        <v>430</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>440</v>
+        <v>431</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>441</v>
+        <v>432</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>443</v>
+        <v>434</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
-        <v>434</v>
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -5639,102 +5550,102 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>445</v>
+        <v>436</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>446</v>
+        <v>437</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>447</v>
+        <v>438</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>453</v>
+        <v>444</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>456</v>
+        <v>447</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>457</v>
+        <v>448</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>458</v>
+        <v>449</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>459</v>
+        <v>450</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>460</v>
+        <v>451</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>461</v>
+        <v>452</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>462</v>
+        <v>453</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>463</v>
+        <v>454</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>464</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>
@@ -5766,226 +5677,226 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>465</v>
+        <v>456</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>466</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>469</v>
+        <v>460</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>470</v>
+        <v>461</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>471</v>
+        <v>462</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>472</v>
+        <v>463</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>473</v>
+        <v>464</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>474</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>475</v>
+        <v>466</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>476</v>
+        <v>467</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>477</v>
+        <v>468</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>478</v>
+        <v>469</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>479</v>
+        <v>470</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>480</v>
+        <v>471</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>481</v>
+        <v>472</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>482</v>
+        <v>473</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>483</v>
+        <v>474</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>484</v>
+        <v>475</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>485</v>
+        <v>476</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>486</v>
+        <v>477</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>487</v>
+        <v>478</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>488</v>
+        <v>479</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>489</v>
+        <v>480</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>490</v>
+        <v>481</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
-        <v>491</v>
+        <v>482</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>492</v>
+        <v>483</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
-        <v>493</v>
+        <v>484</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>494</v>
+        <v>485</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
-        <v>467</v>
+        <v>458</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>468</v>
+        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -6013,12 +5924,12 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>495</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -6042,42 +5953,42 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>498</v>
+        <v>489</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>500</v>
+        <v>491</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>501</v>
+        <v>492</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>502</v>
+        <v>493</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>503</v>
+        <v>494</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>499</v>
+        <v>490</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>504</v>
+        <v>495</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
@@ -6102,12 +6013,12 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>505</v>
+        <v>496</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>506</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -6134,12 +6045,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -6401,12 +6312,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -6656,12 +6567,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
@@ -6833,12 +6744,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
@@ -7043,12 +6954,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">

</xml_diff>

<commit_message>
EPBDS-7113 OpenLUserRuntimeException is user's expected errors.
This exception can be thrown from OpenL rules by calling error("Some message") only.
All other ways are prohibited.
OpenL rules does not support exception handling inside rules, so error(Throwable) method is redudant.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" firstSheet="10" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="MaxMinTests" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,12 @@
     <sheet name="arrays" sheetId="24" r:id="rId24"/>
     <sheet name="alliases" sheetId="25" r:id="rId25"/>
   </sheets>
-  <calcPr calcId="0" iterate="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="500">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="498">
   <si>
     <t>Tests to test rules helper methods for Max and Min value of different types</t>
   </si>
@@ -601,13 +601,7 @@
     <t>return format(num);</t>
   </si>
   <si>
-    <t>Method void testErrorThrowable(Throwable e) throws Throwable</t>
-  </si>
-  <si>
     <t>Method String formatDoubleWithFrm(double num, String format)</t>
-  </si>
-  <si>
-    <t>return error(e);</t>
   </si>
   <si>
     <t>return format(num, format);</t>
@@ -1734,13 +1728,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2135,12 +2129,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="17" t="s">
@@ -2152,10 +2146,10 @@
       <c r="G3" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="16"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
@@ -2164,10 +2158,10 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="16"/>
+      <c r="G6" s="18"/>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2260,10 +2254,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="16"/>
+      <c r="D14" s="18"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
@@ -2272,10 +2266,10 @@
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="16" t="s">
+      <c r="F15" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="16"/>
+      <c r="G15" s="18"/>
       <c r="I15" s="2" t="s">
         <v>21</v>
       </c>
@@ -2368,10 +2362,10 @@
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="16" t="s">
+      <c r="C23" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="16"/>
+      <c r="D23" s="18"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
@@ -2380,10 +2374,10 @@
       <c r="D24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="16"/>
+      <c r="G24" s="18"/>
       <c r="I24" s="2" t="s">
         <v>30</v>
       </c>
@@ -2468,10 +2462,10 @@
       </c>
     </row>
     <row r="32" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C32" s="16" t="s">
+      <c r="C32" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="16"/>
+      <c r="D32" s="18"/>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="1" t="s">
@@ -2480,10 +2474,10 @@
       <c r="D33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F33" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="16"/>
+      <c r="G33" s="18"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="1" t="s">
@@ -2556,10 +2550,10 @@
       </c>
     </row>
     <row r="41" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="16"/>
+      <c r="D41" s="18"/>
     </row>
     <row r="42" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
@@ -2568,10 +2562,10 @@
       <c r="D42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="16" t="s">
+      <c r="F42" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G42" s="16"/>
+      <c r="G42" s="18"/>
     </row>
     <row r="43" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
@@ -2644,10 +2638,10 @@
       </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C50" s="16" t="s">
+      <c r="C50" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="16"/>
+      <c r="D50" s="18"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
@@ -2656,10 +2650,10 @@
       <c r="D51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F51" s="16" t="s">
+      <c r="F51" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="G51" s="16"/>
+      <c r="G51" s="18"/>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
@@ -2741,10 +2735,10 @@
       <c r="G60" s="17"/>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="16" t="s">
+      <c r="C62" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="D62" s="16"/>
+      <c r="D62" s="18"/>
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
@@ -2753,10 +2747,10 @@
       <c r="D63" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="16" t="s">
+      <c r="F63" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G63" s="16"/>
+      <c r="G63" s="18"/>
       <c r="I63" s="2" t="s">
         <v>49</v>
       </c>
@@ -2849,10 +2843,10 @@
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C71" s="16" t="s">
+      <c r="C71" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="D71" s="16"/>
+      <c r="D71" s="18"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
@@ -2861,10 +2855,10 @@
       <c r="D72" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F72" s="16" t="s">
+      <c r="F72" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="G72" s="16"/>
+      <c r="G72" s="18"/>
       <c r="I72" s="2" t="s">
         <v>56</v>
       </c>
@@ -2957,10 +2951,10 @@
       </c>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C80" s="16" t="s">
+      <c r="C80" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D80" s="16"/>
+      <c r="D80" s="18"/>
     </row>
     <row r="81" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C81" s="1" t="s">
@@ -2969,10 +2963,10 @@
       <c r="D81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F81" s="16" t="s">
+      <c r="F81" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="G81" s="16"/>
+      <c r="G81" s="18"/>
       <c r="I81" s="2" t="s">
         <v>61</v>
       </c>
@@ -3057,10 +3051,10 @@
       </c>
     </row>
     <row r="89" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C89" s="16" t="s">
+      <c r="C89" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="D89" s="16"/>
+      <c r="D89" s="18"/>
     </row>
     <row r="90" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C90" s="1" t="s">
@@ -3069,10 +3063,10 @@
       <c r="D90" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F90" s="16" t="s">
+      <c r="F90" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G90" s="16"/>
+      <c r="G90" s="18"/>
     </row>
     <row r="91" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C91" s="1" t="s">
@@ -3145,10 +3139,10 @@
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C98" s="16" t="s">
+      <c r="C98" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D98" s="16"/>
+      <c r="D98" s="18"/>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
@@ -3157,10 +3151,10 @@
       <c r="D99" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F99" s="16" t="s">
+      <c r="F99" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="G99" s="16"/>
+      <c r="G99" s="18"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C100" s="1" t="s">
@@ -3233,10 +3227,10 @@
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C107" s="16" t="s">
+      <c r="C107" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D107" s="16"/>
+      <c r="D107" s="18"/>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" s="1" t="s">
@@ -3245,10 +3239,10 @@
       <c r="D108" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F108" s="16" t="s">
+      <c r="F108" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="G108" s="16"/>
+      <c r="G108" s="18"/>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C109" s="1" t="s">
@@ -3322,26 +3316,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="C80:D80"/>
     <mergeCell ref="C107:D107"/>
     <mergeCell ref="F108:G108"/>
     <mergeCell ref="F81:G81"/>
@@ -3349,6 +3323,26 @@
     <mergeCell ref="F90:G90"/>
     <mergeCell ref="C98:D98"/>
     <mergeCell ref="F99:G99"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="C80:D80"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3373,111 +3367,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>215</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="16" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C7" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C10" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C16" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C22" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3507,127 +3501,127 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>229</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D7" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D10" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D13" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="19" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D19" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D24" s="2" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D25" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D27" s="2" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="28" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D28" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -3656,12 +3650,12 @@
   <sheetData>
     <row r="7" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3687,12 +3681,12 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
@@ -3700,12 +3694,12 @@
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
@@ -3713,12 +3707,12 @@
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
@@ -3726,12 +3720,12 @@
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
@@ -3739,12 +3733,12 @@
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
@@ -3752,12 +3746,12 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
@@ -3765,12 +3759,12 @@
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
@@ -3778,12 +3772,12 @@
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
@@ -3791,12 +3785,12 @@
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
@@ -3804,12 +3798,12 @@
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
@@ -3817,12 +3811,12 @@
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
@@ -3830,12 +3824,12 @@
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
@@ -3843,12 +3837,12 @@
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
@@ -3856,12 +3850,12 @@
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
@@ -3869,12 +3863,12 @@
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
@@ -3882,12 +3876,12 @@
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="9" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
@@ -3895,12 +3889,12 @@
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
@@ -3908,12 +3902,12 @@
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
@@ -3921,12 +3915,12 @@
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" s="9" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" s="10" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
@@ -3934,12 +3928,12 @@
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" s="9" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" s="10" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
@@ -3947,12 +3941,12 @@
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" s="9" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" s="10" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
@@ -3960,12 +3954,12 @@
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" s="9" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" s="10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="67" spans="2:2" x14ac:dyDescent="0.25">
@@ -3973,172 +3967,172 @@
     </row>
     <row r="68" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B68" s="9" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="69" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B69" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="71" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B71" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="74" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B74" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="75" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B75" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="77" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B77" s="9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="78" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B78" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="80" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B80" s="9" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="81" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B81" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="83" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B83" s="9" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="84" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B84" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="86" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B86" s="9" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="87" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B87" s="10" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="89" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B89" s="9" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="90" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B90" s="10" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="92" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B92" s="9" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="93" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B93" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="95" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B95" s="9" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="96" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B96" s="10" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="98" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B98" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="99" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B99" s="10" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="101" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B101" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="102" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B102" s="10" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="104" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B104" s="9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="105" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B105" s="10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="107" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B107" s="9" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="108" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B108" s="10" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="110" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B110" s="9" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="111" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B111" s="10" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B113" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="114" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B114" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="116" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B116" s="9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="117" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B117" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
   </sheetData>
@@ -4166,20 +4160,20 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C2" s="12"/>
       <c r="D2" s="9" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C3" s="12"/>
       <c r="D3" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -4189,20 +4183,20 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C5" s="12"/>
       <c r="D5" s="9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C6" s="12"/>
       <c r="D6" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
@@ -4212,20 +4206,20 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C8" s="12"/>
       <c r="D8" s="9" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C9" s="12"/>
       <c r="D9" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
@@ -4235,20 +4229,20 @@
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C11" s="12"/>
       <c r="D11" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
@@ -4258,20 +4252,20 @@
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C14" s="12"/>
       <c r="D14" s="9" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
@@ -4281,20 +4275,20 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C17" s="12"/>
       <c r="D17" s="9" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C18" s="12"/>
       <c r="D18" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -4305,13 +4299,13 @@
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C20" s="12"/>
       <c r="D20" s="9" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C21" s="12"/>
       <c r="D21" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -4321,13 +4315,13 @@
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" s="12"/>
       <c r="D23" s="9" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" s="12"/>
       <c r="D24" s="10" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
   </sheetData>
@@ -4344,7 +4338,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4355,12 +4351,12 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -4390,92 +4386,92 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>
@@ -4507,162 +4503,162 @@
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="10" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -4694,186 +4690,186 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" s="9" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" s="9" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
   </sheetData>
@@ -4903,92 +4899,92 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
   </sheetData>
@@ -5023,12 +5019,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -5246,146 +5242,146 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
   </sheetData>
@@ -5415,112 +5411,112 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -5550,102 +5546,102 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
     </row>
     <row r="12" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="15" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -5677,226 +5673,226 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="9" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="9" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -5924,12 +5920,12 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
     </row>
   </sheetData>
@@ -5953,42 +5949,42 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="14" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" s="13" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" s="13" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" s="13" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="9" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="13" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
     </row>
     <row r="14" spans="2:2" x14ac:dyDescent="0.25">
@@ -6013,12 +6009,12 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="10" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
     </row>
   </sheetData>
@@ -6045,12 +6041,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -6312,12 +6308,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -6567,12 +6563,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
@@ -6744,12 +6740,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
@@ -6885,8 +6881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:D7"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6914,20 +6910,15 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
+    <row r="5" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="7" t="s">
         <v>187</v>
       </c>
-      <c r="D6" s="7" t="s">
+    </row>
+    <row r="7" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="8" t="s">
         <v>188</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -6954,187 +6945,187 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>191</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="16" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EPBDS-7129 Use floating point result for Median and Avg methods.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -4,41 +4,41 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" activeTab="7"/>
+    <workbookView activeTab="7" windowHeight="8130" windowWidth="16380" xWindow="0" yWindow="60"/>
   </bookViews>
   <sheets>
-    <sheet name="MaxMinTests" sheetId="1" r:id="rId1"/>
-    <sheet name="Mod" sheetId="2" r:id="rId2"/>
-    <sheet name="Slice" sheetId="3" r:id="rId3"/>
-    <sheet name="Sort" sheetId="4" r:id="rId4"/>
-    <sheet name="Contains" sheetId="5" r:id="rId5"/>
-    <sheet name="IndexOf" sheetId="6" r:id="rId6"/>
-    <sheet name="noNulls" sheetId="7" r:id="rId7"/>
-    <sheet name="error and format" sheetId="8" r:id="rId8"/>
-    <sheet name="Quotient" sheetId="9" r:id="rId9"/>
-    <sheet name="Sum" sheetId="10" r:id="rId10"/>
-    <sheet name="Avg" sheetId="11" r:id="rId11"/>
-    <sheet name="logical functions" sheetId="12" r:id="rId12"/>
-    <sheet name="Differents" sheetId="13" r:id="rId13"/>
-    <sheet name="Product" sheetId="14" r:id="rId14"/>
-    <sheet name="Logical" sheetId="15" r:id="rId15"/>
-    <sheet name="Round" sheetId="16" r:id="rId16"/>
-    <sheet name="MaxMinTests2" sheetId="17" r:id="rId17"/>
-    <sheet name="Add" sheetId="18" r:id="rId18"/>
-    <sheet name="AddAll" sheetId="19" r:id="rId19"/>
-    <sheet name="Remove" sheetId="20" r:id="rId20"/>
-    <sheet name="Empty" sheetId="21" r:id="rId21"/>
-    <sheet name="Sheet22" sheetId="22" r:id="rId22"/>
-    <sheet name="small and big" sheetId="23" r:id="rId23"/>
-    <sheet name="arrays" sheetId="24" r:id="rId24"/>
-    <sheet name="alliases" sheetId="25" r:id="rId25"/>
+    <sheet name="MaxMinTests" r:id="rId1" sheetId="1"/>
+    <sheet name="Mod" r:id="rId2" sheetId="2"/>
+    <sheet name="Slice" r:id="rId3" sheetId="3"/>
+    <sheet name="Sort" r:id="rId4" sheetId="4"/>
+    <sheet name="Contains" r:id="rId5" sheetId="5"/>
+    <sheet name="IndexOf" r:id="rId6" sheetId="6"/>
+    <sheet name="noNulls" r:id="rId7" sheetId="7"/>
+    <sheet name="error and format" r:id="rId8" sheetId="8"/>
+    <sheet name="Quotient" r:id="rId9" sheetId="9"/>
+    <sheet name="Sum" r:id="rId10" sheetId="10"/>
+    <sheet name="Avg" r:id="rId11" sheetId="11"/>
+    <sheet name="logical functions" r:id="rId12" sheetId="12"/>
+    <sheet name="Differents" r:id="rId13" sheetId="13"/>
+    <sheet name="Product" r:id="rId14" sheetId="14"/>
+    <sheet name="Logical" r:id="rId15" sheetId="15"/>
+    <sheet name="Round" r:id="rId16" sheetId="16"/>
+    <sheet name="MaxMinTests2" r:id="rId17" sheetId="17"/>
+    <sheet name="Add" r:id="rId18" sheetId="18"/>
+    <sheet name="AddAll" r:id="rId19" sheetId="19"/>
+    <sheet name="Remove" r:id="rId20" sheetId="20"/>
+    <sheet name="Empty" r:id="rId21" sheetId="21"/>
+    <sheet name="Sheet22" r:id="rId22" sheetId="22"/>
+    <sheet name="small and big" r:id="rId23" sheetId="23"/>
+    <sheet name="arrays" r:id="rId24" sheetId="24"/>
+    <sheet name="alliases" r:id="rId25" sheetId="25"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="507">
   <si>
     <t>Tests to test rules helper methods for Max and Min value of different types</t>
   </si>
@@ -1532,12 +1532,40 @@
   </si>
   <si>
     <t>return instanceOf(a, Number.class);</t>
+  </si>
+  <si>
+    <t>Method BigDecimalValue testAvgBigInteger(BigIntegerValue[] values)</t>
+  </si>
+  <si>
+    <t>Method Double testAvgByteType(byte[] values)</t>
+  </si>
+  <si>
+    <t>Method java.lang.Double testAvgByte(java.lang.Byte[] values)</t>
+  </si>
+  <si>
+    <t>Method Double testAvgIntegerType(int[] values)</t>
+  </si>
+  <si>
+    <t>Method java.lang.Double testAvgInteger(java.lang.Integer[] values)</t>
+  </si>
+  <si>
+    <t>Method Double testAvgLongType(long[] values)</t>
+  </si>
+  <si>
+    <t>Method java.lang.Double testAvgLong(java.lang.Long[] values)</t>
+  </si>
+  <si>
+    <t>Method Double testAvgShortType(short[] values)</t>
+  </si>
+  <si>
+    <t>Method java.lang.Double testAvgShort(java.lang.Short[] values)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1699,52 +1727,52 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="11" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="12" fontId="2" numFmtId="0" xfId="2"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="8" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="9" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="9" fontId="5" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="2" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="10" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" borderId="2" fillId="12" fontId="2" numFmtId="0" xfId="2"/>
+    <xf applyBorder="1" applyFont="1" borderId="2" fillId="11" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="10" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="46" name="20% - Accent5" xfId="0"/>
+    <cellStyle builtinId="31" name="40% - Accent1" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1826,10 +1854,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1987,7 +2015,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1996,13 +2024,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -2012,7 +2040,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -2021,7 +2049,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2030,7 +2058,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -2040,12 +2068,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -2076,7 +2104,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -2095,7 +2123,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -2107,25 +2135,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I114"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J114"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="F6" sqref="F6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.5703125"/>
-    <col min="3" max="3" width="19.5703125"/>
-    <col min="4" max="4" width="38.42578125"/>
-    <col min="5" max="5" width="9.5703125"/>
-    <col min="6" max="6" width="28.85546875"/>
-    <col min="7" max="7" width="38.42578125"/>
-    <col min="8" max="8" width="9.5703125"/>
-    <col min="9" max="9" width="72.85546875"/>
-    <col min="10" max="10" width="27.28515625"/>
-    <col min="11" max="1025" width="9.5703125"/>
+    <col min="1" max="2" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" width="19.5703125" collapsed="true"/>
+    <col min="4" max="4" width="38.42578125" collapsed="true"/>
+    <col min="5" max="5" width="9.5703125" collapsed="true"/>
+    <col min="6" max="6" width="28.85546875" collapsed="true"/>
+    <col min="7" max="7" width="38.42578125" collapsed="true"/>
+    <col min="8" max="8" width="9.5703125" collapsed="true"/>
+    <col min="9" max="9" width="72.85546875" collapsed="true"/>
+    <col min="10" max="10" width="27.28515625" collapsed="true"/>
+    <col min="11" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3344,26 +3372,26 @@
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="C14:D14"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.5703125"/>
-    <col min="3" max="3" width="78.7109375"/>
-    <col min="4" max="4" width="9.5703125"/>
-    <col min="5" max="5" width="78.7109375"/>
-    <col min="6" max="1025" width="9.5703125"/>
+    <col min="1" max="2" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" width="78.7109375" collapsed="true"/>
+    <col min="4" max="4" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" width="78.7109375" collapsed="true"/>
+    <col min="6" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -3478,26 +3506,26 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="9.5703125"/>
-    <col min="4" max="4" width="62.42578125"/>
-    <col min="5" max="5" width="9.5703125"/>
-    <col min="6" max="6" width="62.42578125"/>
-    <col min="7" max="1025" width="9.5703125"/>
+    <col min="1" max="3" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" width="62.42578125" collapsed="true"/>
+    <col min="5" max="5" width="9.5703125" collapsed="true"/>
+    <col min="6" max="6" width="62.42578125" collapsed="true"/>
+    <col min="7" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -3513,7 +3541,7 @@
         <v>228</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>229</v>
+        <v>500</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3526,10 +3554,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D9" s="2" t="s">
-        <v>231</v>
+        <v>498</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>232</v>
+        <v>506</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3542,10 +3570,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D12" s="2" t="s">
-        <v>233</v>
+        <v>499</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>234</v>
+        <v>502</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -3558,10 +3586,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D15" s="2" t="s">
-        <v>235</v>
+        <v>505</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>236</v>
+        <v>504</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -3574,7 +3602,7 @@
     </row>
     <row r="18" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D18" s="2" t="s">
-        <v>237</v>
+        <v>501</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>238</v>
@@ -3590,7 +3618,7 @@
     </row>
     <row r="21" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D21" s="2" t="s">
-        <v>239</v>
+        <v>503</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>240</v>
@@ -3628,24 +3656,24 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C7:C8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C7:D8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.5703125"/>
-    <col min="3" max="3" width="38.85546875"/>
-    <col min="4" max="1025" width="9.5703125"/>
+    <col min="1" max="2" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" width="38.85546875" collapsed="true"/>
+    <col min="4" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="7" spans="3:3" x14ac:dyDescent="0.25">
@@ -3659,24 +3687,24 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B117"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C117"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B118" sqref="B118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125"/>
-    <col min="2" max="2" width="82.42578125"/>
-    <col min="3" max="1025" width="9.5703125"/>
+    <col min="1" max="1" width="9.5703125" collapsed="true"/>
+    <col min="2" max="2" width="82.42578125" collapsed="true"/>
+    <col min="3" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
@@ -4136,26 +4164,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.28515625"/>
-    <col min="2" max="2" width="45.85546875"/>
-    <col min="3" max="3" width="10.28515625"/>
-    <col min="4" max="4" width="39"/>
-    <col min="5" max="1025" width="10.28515625"/>
+    <col min="1" max="1" width="10.28515625" collapsed="true"/>
+    <col min="2" max="2" width="45.85546875" collapsed="true"/>
+    <col min="3" max="3" width="10.28515625" collapsed="true"/>
+    <col min="4" max="4" width="39.0" collapsed="true"/>
+    <col min="5" max="1025" width="10.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -4325,8 +4353,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4335,18 +4363,18 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="49.28515625"/>
-    <col min="3" max="1012" width="11.5703125"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="49.28515625" collapsed="true"/>
+    <col min="3" max="1012" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -4360,8 +4388,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4370,18 +4398,18 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="51.28515625"/>
-    <col min="3" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="51.28515625" collapsed="true"/>
+    <col min="3" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -4475,8 +4503,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4485,20 +4513,20 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E31"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="50.28515625"/>
-    <col min="3" max="3" width="11.5703125"/>
-    <col min="4" max="4" width="56.42578125"/>
-    <col min="5" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="50.28515625" collapsed="true"/>
+    <col min="3" max="3" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" width="56.42578125" collapsed="true"/>
+    <col min="5" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -4662,8 +4690,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4672,20 +4700,20 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D48"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="70.140625"/>
-    <col min="3" max="3" width="11.5703125"/>
-    <col min="4" max="4" width="68"/>
-    <col min="5" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="70.140625" collapsed="true"/>
+    <col min="3" max="3" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" width="68.0" collapsed="true"/>
+    <col min="5" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -4873,8 +4901,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4883,18 +4911,18 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="56.42578125"/>
-    <col min="3" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="56.42578125" collapsed="true"/>
+    <col min="3" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
@@ -4988,8 +5016,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4998,24 +5026,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125"/>
-    <col min="2" max="2" width="9.5703125"/>
-    <col min="3" max="3" width="72.85546875"/>
-    <col min="4" max="4" width="9.5703125"/>
-    <col min="5" max="5" width="72.85546875"/>
-    <col min="6" max="6" width="9.5703125"/>
-    <col min="7" max="7" width="19.5703125"/>
-    <col min="8" max="8" width="38.42578125"/>
-    <col min="9" max="1025" width="9.5703125"/>
+    <col min="1" max="1" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" width="72.85546875" collapsed="true"/>
+    <col min="4" max="4" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" width="72.85546875" collapsed="true"/>
+    <col min="6" max="6" width="9.5703125" collapsed="true"/>
+    <col min="7" max="7" width="19.5703125" collapsed="true"/>
+    <col min="8" max="8" width="38.42578125" collapsed="true"/>
+    <col min="9" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -5218,26 +5246,26 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="53.42578125"/>
-    <col min="3" max="3" width="11.5703125"/>
-    <col min="4" max="4" width="57.5703125"/>
-    <col min="5" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="53.42578125" collapsed="true"/>
+    <col min="3" max="3" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" width="57.5703125" collapsed="true"/>
+    <col min="5" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -5385,8 +5413,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5395,18 +5423,18 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="62.28515625"/>
-    <col min="3" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="62.28515625" collapsed="true"/>
+    <col min="3" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
@@ -5520,8 +5548,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5530,18 +5558,18 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C30"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="78.85546875"/>
-    <col min="3" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="78.85546875" collapsed="true"/>
+    <col min="3" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
@@ -5645,8 +5673,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5655,20 +5683,20 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:E42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125"/>
-    <col min="2" max="2" width="50"/>
-    <col min="3" max="3" width="11.5703125"/>
-    <col min="4" max="4" width="65.42578125"/>
-    <col min="5" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" width="50.0" collapsed="true"/>
+    <col min="3" max="3" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" width="65.42578125" collapsed="true"/>
+    <col min="5" max="1025" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
@@ -5896,8 +5924,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.78749999999999998" header="0.78749999999999998" left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5906,8 +5934,8 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
@@ -5915,7 +5943,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="51.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
@@ -5929,13 +5957,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
@@ -5943,8 +5971,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="51.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="53.7109375" customWidth="1"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="51.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="53.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.25">
@@ -6018,26 +6046,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125"/>
-    <col min="2" max="2" width="9.5703125"/>
-    <col min="3" max="3" width="72.85546875"/>
-    <col min="4" max="4" width="9.5703125"/>
-    <col min="5" max="5" width="72.85546875"/>
-    <col min="6" max="1025" width="9.5703125"/>
+    <col min="1" max="1" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" width="72.85546875" collapsed="true"/>
+    <col min="4" max="4" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" width="72.85546875" collapsed="true"/>
+    <col min="6" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -6284,27 +6312,27 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125"/>
-    <col min="2" max="2" width="9.5703125"/>
-    <col min="3" max="3" width="72.85546875"/>
-    <col min="4" max="4" width="9.5703125"/>
-    <col min="5" max="5" width="72.85546875"/>
-    <col min="6" max="1025" width="9.5703125"/>
+    <col min="1" max="1" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" width="72.85546875" collapsed="true"/>
+    <col min="4" max="4" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" width="72.85546875" collapsed="true"/>
+    <col min="6" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -6539,27 +6567,27 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125"/>
-    <col min="2" max="2" width="9.5703125"/>
-    <col min="3" max="3" width="82.42578125"/>
-    <col min="4" max="4" width="9.5703125"/>
-    <col min="5" max="5" width="93.28515625"/>
-    <col min="6" max="1025" width="9.5703125"/>
+    <col min="1" max="1" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" width="82.42578125" collapsed="true"/>
+    <col min="4" max="4" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" width="93.28515625" collapsed="true"/>
+    <col min="6" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -6718,25 +6746,25 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125"/>
-    <col min="2" max="2" width="9.5703125"/>
-    <col min="3" max="3" width="82.42578125"/>
-    <col min="4" max="1025" width="9.5703125"/>
+    <col min="1" max="1" width="10.42578125" collapsed="true"/>
+    <col min="2" max="2" width="9.5703125" collapsed="true"/>
+    <col min="3" max="3" width="82.42578125" collapsed="true"/>
+    <col min="4" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -6841,24 +6869,24 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125"/>
-    <col min="2" max="2" width="82.42578125"/>
-    <col min="3" max="1025" width="9.5703125"/>
+    <col min="1" max="1" width="9.5703125" collapsed="true"/>
+    <col min="2" max="2" width="82.42578125" collapsed="true"/>
+    <col min="3" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
@@ -6872,26 +6900,26 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125"/>
-    <col min="2" max="2" width="82.42578125"/>
-    <col min="3" max="3" width="9.5703125"/>
-    <col min="4" max="4" width="82.42578125"/>
-    <col min="5" max="1025" width="9.5703125"/>
+    <col min="1" max="1" width="9.5703125" collapsed="true"/>
+    <col min="2" max="2" width="82.42578125" collapsed="true"/>
+    <col min="3" max="3" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" width="82.42578125" collapsed="true"/>
+    <col min="5" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -6910,38 +6938,38 @@
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="5" spans="2:4" thickBot="1" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="6" spans="2:4" thickBot="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D6" s="7" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="7" spans="2:4" thickBot="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="D7" s="8" t="s">
         <v>188</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125"/>
-    <col min="2" max="2" width="72.85546875"/>
-    <col min="3" max="3" width="9.5703125"/>
-    <col min="4" max="4" width="72.85546875"/>
-    <col min="5" max="1025" width="9.5703125"/>
+    <col min="1" max="1" width="9.5703125" collapsed="true"/>
+    <col min="2" max="2" width="72.85546875" collapsed="true"/>
+    <col min="3" max="3" width="9.5703125" collapsed="true"/>
+    <col min="4" max="4" width="72.85546875" collapsed="true"/>
+    <col min="5" max="1025" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -7132,7 +7160,7 @@
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins bottom="0.75" footer="0.51180555555555496" header="0.51180555555555496" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup copies="0" firstPageNumber="0" horizontalDpi="0" orientation="portrait" paperSize="0" scale="0" usePrinterDefaults="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
EPBDS-7699 Nullsafety doesn't work with DobleValues for avg() function
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pvlad\Documents\EIS\OpenL\openl-pub\DEV\org.openl.rules\test\rules\helpers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\test\rules\helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D1D75D13-D9C7-49E1-8AB2-C9E8443B4E5B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" tabRatio="891" firstSheet="7" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" tabRatio="891" firstSheet="8" activeTab="25" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MaxMinTests" sheetId="1" r:id="rId1"/>
@@ -1510,9 +1511,6 @@
     <t>Method Double testMedianDouble(Double[] values)</t>
   </si>
   <si>
-    <t>Method BigInteger testMedianBigInteger(BigInteger[] values)</t>
-  </si>
-  <si>
     <t>Method BigDecimal testMedianBigDecimal(BigDecimal[] values)</t>
   </si>
   <si>
@@ -1841,12 +1839,15 @@
   </si>
   <si>
     <t>Method Short[] testShortRemove(Short[] inArr,int pos)</t>
+  </si>
+  <si>
+    <t>Method BigDecimal testMedianBigInteger(BigInteger[] values)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2038,13 +2039,13 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2210,6 +2211,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2245,6 +2263,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -2420,7 +2455,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK114"/>
   <sheetViews>
     <sheetView topLeftCell="F19" zoomScaleNormal="100" workbookViewId="0">
@@ -2442,12 +2477,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="17" t="s">
@@ -2459,10 +2494,10 @@
       <c r="G3" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="16"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
@@ -2471,10 +2506,10 @@
       <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="18" t="s">
+      <c r="F6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="G6" s="18"/>
+      <c r="G6" s="16"/>
       <c r="I6" s="2" t="s">
         <v>6</v>
       </c>
@@ -2567,10 +2602,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C14" s="18" t="s">
+      <c r="C14" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="18"/>
+      <c r="D14" s="16"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
@@ -2579,10 +2614,10 @@
       <c r="D15" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="18" t="s">
+      <c r="F15" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="18"/>
+      <c r="G15" s="16"/>
       <c r="I15" s="2" t="s">
         <v>21</v>
       </c>
@@ -2675,10 +2710,10 @@
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C23" s="18" t="s">
+      <c r="C23" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D23" s="18"/>
+      <c r="D23" s="16"/>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" s="1" t="s">
@@ -2687,10 +2722,10 @@
       <c r="D24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="18"/>
+      <c r="G24" s="16"/>
       <c r="I24" s="2" t="s">
         <v>30</v>
       </c>
@@ -2783,10 +2818,10 @@
       </c>
     </row>
     <row r="32" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="18"/>
+      <c r="D32" s="16"/>
     </row>
     <row r="33" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
@@ -2795,10 +2830,10 @@
       <c r="D33" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F33" s="18" t="s">
+      <c r="F33" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G33" s="18"/>
+      <c r="G33" s="16"/>
       <c r="I33" s="2" t="s">
         <v>477</v>
       </c>
@@ -2877,10 +2912,10 @@
       </c>
     </row>
     <row r="41" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="18" t="s">
+      <c r="C41" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="18"/>
+      <c r="D41" s="16"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C42" s="1" t="s">
@@ -2889,10 +2924,10 @@
       <c r="D42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="18" t="s">
+      <c r="F42" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="G42" s="18"/>
+      <c r="G42" s="16"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C43" s="1" t="s">
@@ -2965,10 +3000,10 @@
       </c>
     </row>
     <row r="50" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D50" s="18"/>
+      <c r="D50" s="16"/>
     </row>
     <row r="51" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C51" s="1" t="s">
@@ -2977,10 +3012,10 @@
       <c r="D51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F51" s="18" t="s">
+      <c r="F51" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="G51" s="18"/>
+      <c r="G51" s="16"/>
     </row>
     <row r="52" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C52" s="1" t="s">
@@ -3062,10 +3097,10 @@
       <c r="G60" s="17"/>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C62" s="18" t="s">
+      <c r="C62" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D62" s="18"/>
+      <c r="D62" s="16"/>
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
@@ -3074,10 +3109,10 @@
       <c r="D63" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="18" t="s">
+      <c r="F63" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="G63" s="18"/>
+      <c r="G63" s="16"/>
       <c r="I63" s="2" t="s">
         <v>49</v>
       </c>
@@ -3170,10 +3205,10 @@
       </c>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C71" s="18" t="s">
+      <c r="C71" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="D71" s="18"/>
+      <c r="D71" s="16"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C72" s="1" t="s">
@@ -3182,10 +3217,10 @@
       <c r="D72" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F72" s="18" t="s">
+      <c r="F72" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="G72" s="18"/>
+      <c r="G72" s="16"/>
       <c r="I72" s="2" t="s">
         <v>56</v>
       </c>
@@ -3278,10 +3313,10 @@
       </c>
     </row>
     <row r="80" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C80" s="18" t="s">
+      <c r="C80" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D80" s="18"/>
+      <c r="D80" s="16"/>
     </row>
     <row r="81" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C81" s="1" t="s">
@@ -3290,10 +3325,10 @@
       <c r="D81" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F81" s="18" t="s">
+      <c r="F81" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G81" s="18"/>
+      <c r="G81" s="16"/>
       <c r="I81" s="2" t="s">
         <v>61</v>
       </c>
@@ -3386,10 +3421,10 @@
       </c>
     </row>
     <row r="89" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C89" s="18" t="s">
+      <c r="C89" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D89" s="18"/>
+      <c r="D89" s="16"/>
     </row>
     <row r="90" spans="3:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C90" s="1" t="s">
@@ -3398,10 +3433,10 @@
       <c r="D90" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F90" s="18" t="s">
+      <c r="F90" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="G90" s="18"/>
+      <c r="G90" s="16"/>
       <c r="I90" s="2" t="s">
         <v>475</v>
       </c>
@@ -3480,10 +3515,10 @@
       </c>
     </row>
     <row r="98" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C98" s="18" t="s">
+      <c r="C98" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D98" s="18"/>
+      <c r="D98" s="16"/>
     </row>
     <row r="99" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C99" s="1" t="s">
@@ -3492,10 +3527,10 @@
       <c r="D99" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F99" s="18" t="s">
+      <c r="F99" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G99" s="18"/>
+      <c r="G99" s="16"/>
     </row>
     <row r="100" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C100" s="1" t="s">
@@ -3568,10 +3603,10 @@
       </c>
     </row>
     <row r="107" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C107" s="18" t="s">
+      <c r="C107" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D107" s="18"/>
+      <c r="D107" s="16"/>
     </row>
     <row r="108" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C108" s="1" t="s">
@@ -3580,10 +3615,10 @@
       <c r="D108" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F108" s="18" t="s">
+      <c r="F108" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="G108" s="18"/>
+      <c r="G108" s="16"/>
     </row>
     <row r="109" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C109" s="1" t="s">
@@ -3657,6 +3692,26 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="C3:G3"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="F51:G51"/>
+    <mergeCell ref="C60:G60"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="F72:G72"/>
+    <mergeCell ref="C80:D80"/>
     <mergeCell ref="C107:D107"/>
     <mergeCell ref="F108:G108"/>
     <mergeCell ref="F81:G81"/>
@@ -3664,26 +3719,6 @@
     <mergeCell ref="F90:G90"/>
     <mergeCell ref="C98:D98"/>
     <mergeCell ref="F99:G99"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="F72:G72"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="F51:G51"/>
-    <mergeCell ref="C60:G60"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="C3:G3"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="C14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -3691,7 +3726,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AMK29"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
@@ -3708,12 +3743,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
@@ -3845,7 +3880,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AMK29"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
@@ -3863,12 +3898,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D6" s="2" t="s">
@@ -4011,7 +4046,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A7:AMK8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4042,7 +4077,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A2:AMK126"/>
   <sheetViews>
     <sheetView topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
@@ -4514,32 +4549,32 @@
     </row>
     <row r="119" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B119" s="9" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="120" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B120" s="10" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="122" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B122" s="9" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="123" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B123" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="125" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B125" s="9" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="126" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B126" s="10" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>
@@ -4549,7 +4584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A2:AMK24"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4742,7 +4777,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A3:ALX4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4777,7 +4812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A3:AMK28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4892,7 +4927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A3:AMK37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
@@ -5070,10 +5105,10 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -5086,10 +5121,10 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
@@ -5111,7 +5146,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A2:AMK60"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
@@ -5196,7 +5231,7 @@
         <v>347</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -5212,7 +5247,7 @@
         <v>348</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -5228,7 +5263,7 @@
         <v>349</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -5244,7 +5279,7 @@
         <v>350</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -5260,7 +5295,7 @@
         <v>351</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -5276,7 +5311,7 @@
         <v>352</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -5292,7 +5327,7 @@
         <v>353</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
@@ -5308,7 +5343,7 @@
         <v>354</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
@@ -5324,7 +5359,7 @@
         <v>355</v>
       </c>
       <c r="D38" s="9" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
@@ -5340,7 +5375,7 @@
         <v>356</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
@@ -5356,7 +5391,7 @@
         <v>357</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
@@ -5372,7 +5407,7 @@
         <v>358</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
@@ -5385,15 +5420,15 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B50" s="9" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="10" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D51" s="10" t="s">
         <v>337</v>
@@ -5401,15 +5436,15 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B53" s="9" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B54" s="10" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>340</v>
@@ -5417,7 +5452,7 @@
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D56" s="9" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.25">
@@ -5427,7 +5462,7 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D59" s="9" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
@@ -5446,7 +5481,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A2:AMK27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5467,7 +5502,7 @@
         <v>359</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
@@ -5483,7 +5518,7 @@
         <v>361</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
@@ -5499,7 +5534,7 @@
         <v>362</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
@@ -5515,7 +5550,7 @@
         <v>363</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
@@ -5531,7 +5566,7 @@
         <v>364</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
@@ -5547,7 +5582,7 @@
         <v>365</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -5563,7 +5598,7 @@
         <v>366</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -5579,7 +5614,7 @@
         <v>367</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -5611,7 +5646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK45"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
@@ -5632,12 +5667,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -5837,11 +5872,11 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A2:AMK52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D59" sqref="D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5999,10 +6034,10 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -6015,10 +6050,10 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -6031,10 +6066,10 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
@@ -6047,10 +6082,10 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
@@ -6063,10 +6098,10 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="9" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
@@ -6079,10 +6114,10 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B45" s="9" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
@@ -6095,10 +6130,10 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="9" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
@@ -6111,10 +6146,10 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="9" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
@@ -6136,7 +6171,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A2:AMK33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6271,7 +6306,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="A2:AMK30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6396,7 +6431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A2:AMK42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -6647,7 +6682,7 @@
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="B2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6675,7 +6710,7 @@
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="B2:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6764,11 +6799,11 @@
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="B1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6784,7 +6819,7 @@
         <v>482</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="3" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6801,7 +6836,7 @@
         <v>484</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="6" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6818,7 +6853,7 @@
         <v>485</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6835,7 +6870,7 @@
         <v>486</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6849,10 +6884,10 @@
     <row r="13" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="15" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6869,7 +6904,7 @@
         <v>487</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6883,7 +6918,7 @@
     <row r="19" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
-        <v>488</v>
+        <v>598</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6894,7 +6929,7 @@
     <row r="22" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -6909,7 +6944,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK50"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
@@ -6927,12 +6962,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -7176,7 +7211,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7194,12 +7229,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C4" s="2" t="s">
@@ -7431,7 +7466,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMK57"/>
   <sheetViews>
     <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
@@ -7451,12 +7486,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
@@ -7476,10 +7511,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C6" s="2" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -7492,10 +7527,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C9" s="2" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -7508,10 +7543,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -7524,10 +7559,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -7540,10 +7575,10 @@
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
@@ -7556,10 +7591,10 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
@@ -7572,10 +7607,10 @@
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C24" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
@@ -7588,10 +7623,10 @@
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
@@ -7605,10 +7640,10 @@
     <row r="30" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="2" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="32" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7622,10 +7657,10 @@
     <row r="33" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="35" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7639,10 +7674,10 @@
     <row r="36" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="37" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="38" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7656,10 +7691,10 @@
     <row r="39" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="40" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="41" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7673,10 +7708,10 @@
     <row r="42" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="44" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7690,10 +7725,10 @@
     <row r="45" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="47" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7707,10 +7742,10 @@
     <row r="48" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="50" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7724,10 +7759,10 @@
     <row r="51" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="53" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7741,7 +7776,7 @@
     <row r="54" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="55" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E55" s="2" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="56" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7760,7 +7795,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AMK29"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
@@ -7778,12 +7813,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C3" s="7" t="s">
@@ -7798,10 +7833,10 @@
     <row r="5" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="7" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7815,10 +7850,10 @@
     <row r="8" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9" s="7" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7832,10 +7867,10 @@
     <row r="11" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="7" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7849,10 +7884,10 @@
     <row r="14" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="15" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="7" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7866,10 +7901,10 @@
     <row r="17" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C18" s="7" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="19" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7883,10 +7918,10 @@
     <row r="20" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C21" s="7" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="22" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7900,10 +7935,10 @@
     <row r="23" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="7" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="25" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7917,10 +7952,10 @@
     <row r="26" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="7" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="28" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -7942,7 +7977,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A3:AMK4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -7973,7 +8008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A3:AMK7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8023,7 +8058,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AMK37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -8040,12 +8075,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>165</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">

</xml_diff>

<commit_message>
EPBDS-8318 Improve "contains" function, so it could search a value in range and the array of ranges.
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\test\rules\helpers\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE1696A-7ED3-4950-8200-489D452ABD24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8130" tabRatio="891" activeTab="10"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="891" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mod" sheetId="2" r:id="rId1"/>
@@ -35,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="493">
   <si>
     <t>Tests to test rules helper methods for Mod methods</t>
   </si>
@@ -1466,12 +1472,60 @@
   </si>
   <si>
     <t>Method BigDecimal testMedianBigInteger(BigInteger[] values)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsIntegerTypeInIntRangeArr(IntRange[] searchIn, Integer searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsDoubleTypeInDoubleRangeArr(DoubleRange[] searchIn, Double searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsCharacterTypeInCharRangeArr(CharRange[] searchIn, Character searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsCharacterTypeInCharRangeArr2(CharRange[] searchIn, char searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsDoubleTypeInDoubleRangeArr2(DoubleRange[] searchIn, double searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsIntegerTypeInIntRangeArr2(IntRange[] searchIn, int searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsStringTypeInStringRangeArr(StringRange[] searchIn, String searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsCharSequenceTypeInStringRangeArr(StringRange[] searchIn, CharSequence searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsIntegerArrTypeInIntRangeArr(IntRange[] searchIn, Integer[] searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsIntegerArrTypeInIntRangeArr2(IntRange[] searchIn, int[] searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsDoubleArrTypeInDoubleRangeArr(DoubleRange[] searchIn, Double[] searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsDoubleArrTypeInDoubleRangeArr2(DoubleRange[] searchIn, double[] searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsCharacterArrTypeInCharRangeArr(CharRange[] searchIn, Character[] searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsCharacterArrTypeInCharRangeArr2(CharRange[] searchIn, char[] searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsCharSequenceArrTypeInStringRangeArr(StringRange[] searchIn, CharSequence[] searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsStringArrTypeInStringRangeArr(StringRange[] searchIn, String[] searchFor)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1625,9 +1679,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="20% - Accent5" xfId="2" builtinId="46"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="20% — акцент5" xfId="2" builtinId="46"/>
+    <cellStyle name="40% — акцент1" xfId="1" builtinId="31"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1711,9 +1765,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1751,9 +1805,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1786,9 +1840,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1821,9 +1892,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1996,7 +2084,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK45"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
@@ -2222,7 +2310,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:AMK126"/>
   <sheetViews>
     <sheetView topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
@@ -2729,10 +2817,10 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A3:ALX4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
@@ -2764,7 +2852,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A3:AMK28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2879,7 +2967,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A3:AMK37"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
@@ -3098,7 +3186,7 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A2:AMK60"/>
   <sheetViews>
     <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
@@ -3433,7 +3521,7 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A2:AMK27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3598,7 +3686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A2:AMK52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -3897,7 +3985,7 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A2:AMK33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4032,7 +4120,7 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A2:AMK30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4157,7 +4245,7 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A2:AMK42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -4408,7 +4496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK50"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
@@ -4675,7 +4763,7 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="B2:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4703,7 +4791,7 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="B2:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4792,7 +4880,7 @@
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="B1:D25"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
@@ -4937,7 +5025,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMK52"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5192,11 +5280,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AMK80"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G71" sqref="G71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5355,7 +5443,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="2" t="s">
         <v>85</v>
       </c>
@@ -5363,154 +5451,290 @@
         <v>85</v>
       </c>
     </row>
-    <row r="30" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="29" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>482</v>
+      </c>
+    </row>
     <row r="31" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="1" t="s">
+        <v>478</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C36" s="1" t="s">
+        <v>479</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C39" s="1" t="s">
+        <v>483</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="40" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C42" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="E42" s="1" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="32" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="2" t="s">
+    <row r="43" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C43" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="33" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="1" t="s">
+    <row r="44" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C45" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="35" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="2" t="s">
+    <row r="46" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C46" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="1" t="s">
+    <row r="47" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C48" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="E48" s="1" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="38" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="2" t="s">
+    <row r="49" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C49" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E38" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="40" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="1" t="s">
+    <row r="50" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="51" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C51" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="E51" s="1" t="s">
         <v>401</v>
       </c>
     </row>
-    <row r="41" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="2" t="s">
+    <row r="52" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E52" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="42" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="1" t="s">
+    <row r="53" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C54" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="E54" s="1" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="44" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="2" t="s">
+    <row r="55" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C55" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E55" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="1" t="s">
+    <row r="56" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="E57" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="47" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="2" t="s">
+    <row r="58" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C58" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="1" t="s">
+    <row r="59" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C60" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="E60" s="1" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="50" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="2" t="s">
+    <row r="61" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C61" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E61" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="51" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="52" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="1" t="s">
+    <row r="62" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C63" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="E52" s="1" t="s">
+      <c r="E63" s="1" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="53" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="2" t="s">
+    <row r="64" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C64" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E53" s="2" t="s">
+      <c r="E64" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="54" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E55" s="1" t="s">
+    <row r="65" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="66" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E66" s="1" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="56" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E56" s="2" t="s">
+    <row r="67" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E67" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="57" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C69" s="1" t="s">
+        <v>485</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C70" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C72" s="1" t="s">
+        <v>487</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C73" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="74" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C75" s="1" t="s">
+        <v>489</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="76" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="77" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C78" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="79" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C79" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="80" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
@@ -5521,7 +5745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMK29"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
@@ -5703,7 +5927,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A3:AMK4"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5734,7 +5958,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A3:AMK7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5784,7 +6008,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AMK37"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -5994,7 +6218,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A7:AMK8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
EPBDS-8686 DateRange doesn't work for Smart Rules
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\DEV\org.openl.rules\test\rules\helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EE1696A-7ED3-4950-8200-489D452ABD24}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A991698A-BFFA-4D97-831B-614F0B3D133F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="891" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39930" yWindow="2580" windowWidth="23880" windowHeight="16965" tabRatio="891" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mod" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="496">
   <si>
     <t>Tests to test rules helper methods for Mod methods</t>
   </si>
@@ -1520,6 +1520,15 @@
   </si>
   <si>
     <t>Method boolean testContainsStringArrTypeInStringRangeArr(StringRange[] searchIn, String[] searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsDateArrTypeInDateRangeArr(DateRange[] searchIn, Date[] searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsDateInDateArr(Date[] searchIn, Date searchFor)</t>
+  </si>
+  <si>
+    <t>Method boolean testContainsDateTypeInDateRangeArr(DateRange[] searchIn, Date searchFor)</t>
   </si>
 </sst>
 </file>
@@ -5281,10 +5290,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AMK80"/>
+  <dimension ref="A1:AMK86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G71" sqref="G71"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5734,7 +5743,35 @@
         <v>85</v>
       </c>
     </row>
-    <row r="80" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="81" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C81" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C82" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="84" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C84" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C85" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
EPBDS-12838 copy() operation does not copy transient object fields
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/helpers/RulesUtilsTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\DEV\org.openl.rules\test\rules\helpers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C277A0-DB59-49AC-95C3-53E25EA477C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270B736A-D5C6-4954-8F26-E9081C3B4870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="855" windowWidth="23430" windowHeight="12045" tabRatio="891" firstSheet="6" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3000" yWindow="1245" windowWidth="25695" windowHeight="15825" tabRatio="891" firstSheet="6" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mod" sheetId="2" r:id="rId1"/>
@@ -33,15 +33,16 @@
     <sheet name="Sheet22" sheetId="22" r:id="rId18"/>
     <sheet name="small and big" sheetId="23" r:id="rId19"/>
     <sheet name="arrays" sheetId="24" r:id="rId20"/>
-    <sheet name="alliases" sheetId="25" r:id="rId21"/>
-    <sheet name="median" sheetId="26" r:id="rId22"/>
+    <sheet name="copy" sheetId="27" r:id="rId21"/>
+    <sheet name="alliases" sheetId="25" r:id="rId22"/>
+    <sheet name="median" sheetId="26" r:id="rId23"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="509">
   <si>
     <t>Tests to test rules helper methods for Mod methods</t>
   </si>
@@ -1562,6 +1563,12 @@
   </si>
   <si>
     <t>Method Integer[] testFlatten8(Integer[] x1, Integer[] x2, Integer x3)</t>
+  </si>
+  <si>
+    <t>return copy(o);</t>
+  </si>
+  <si>
+    <t>Method Object copyObject(Object o)</t>
   </si>
 </sst>
 </file>
@@ -4808,7 +4815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="B2:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
@@ -4913,6 +4920,31 @@
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE1D8C4-FDC0-420B-B3B0-C52DFA404187}">
+  <dimension ref="C4:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>507</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="B2:D20"/>
   <sheetViews>
@@ -5001,7 +5033,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <dimension ref="B1:D25"/>
   <sheetViews>

</xml_diff>